<commit_message>
fixed double counting mistake
</commit_message>
<xml_diff>
--- a/data/all_data_df.xlsx
+++ b/data/all_data_df.xlsx
@@ -7336,16 +7336,16 @@
         <v>0</v>
       </c>
       <c r="AL53" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">

</xml_diff>